<commit_message>
excel design db rule
</commit_message>
<xml_diff>
--- a/designdb_rule_formula.xlsx
+++ b/designdb_rule_formula.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halk.atomi\Desktop\Designdb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Loyalty\config-service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED0455-063B-405E-BF27-D6D080AB8694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53410B0-D0EA-4783-A776-65A3840B6A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF300C33-0EAE-4BA3-B905-80901D69EA07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14160" xr2:uid="{AF300C33-0EAE-4BA3-B905-80901D69EA07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="70">
   <si>
     <t>STATUS</t>
   </si>
@@ -205,6 +205,45 @@
   </si>
   <si>
     <t>CF_TRANSACTION_TYPE</t>
+  </si>
+  <si>
+    <t>EXCHANGE_POINT</t>
+  </si>
+  <si>
+    <t>EXCHANGE_VALUE</t>
+  </si>
+  <si>
+    <t>FIX_POINT_AMOUNT</t>
+  </si>
+  <si>
+    <t>FREQUENCY_LIMIT_EVENT_PER_USER</t>
+  </si>
+  <si>
+    <t>FREQUENCY_LIMIT_POINT_PER_USER</t>
+  </si>
+  <si>
+    <t>FREQUENCY_TIME_WAIT</t>
+  </si>
+  <si>
+    <t>IS_EXCHANGE_BY_VALUE</t>
+  </si>
+  <si>
+    <t>IS_NET_VALUE</t>
+  </si>
+  <si>
+    <t>LIMIT_EVENT_PER_USER</t>
+  </si>
+  <si>
+    <t>LIMIT_POINT_PER_TRANSACTION</t>
+  </si>
+  <si>
+    <t>LIMIT_POINT_PER_USER</t>
+  </si>
+  <si>
+    <t>MIN_TRANSACTION</t>
+  </si>
+  <si>
+    <t>TIME_WAIT</t>
   </si>
 </sst>
 </file>
@@ -562,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09E2494-0AE4-49D1-AC85-37E251AD677A}">
-  <dimension ref="B2:D124"/>
+  <dimension ref="B2:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128:D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,6 +1765,226 @@
         <v>6</v>
       </c>
     </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="1">
+        <v>1</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="1">
+        <v>2</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="1">
+        <v>3</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="1">
+        <v>4</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="1">
+        <v>5</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="1">
+        <v>6</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="1">
+        <v>7</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="1">
+        <v>8</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="1">
+        <v>9</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="1">
+        <v>10</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="1">
+        <v>11</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="1">
+        <v>12</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="1">
+        <v>13</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="1">
+        <v>14</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="1">
+        <v>15</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="1">
+        <v>16</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="1">
+        <v>17</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="1">
+        <v>18</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="1">
+        <v>19</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="1">
+        <v>20</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>